<commit_message>
fix(excelreader): trying to fix exceptions
</commit_message>
<xml_diff>
--- a/Data/ExcelBeginner.xlsx
+++ b/Data/ExcelBeginner.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="test" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -73,6 +73,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -132,12 +133,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -267,32 +272,28 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="6.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -300,19 +301,19 @@
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="C2" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -320,26 +321,26 @@
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="2" t="n">
         <v>35</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
feat(dynamic table read): it is now dynamically creating a table and adding the data below the headings
</commit_message>
<xml_diff>
--- a/Data/ExcelBeginner.xlsx
+++ b/Data/ExcelBeginner.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -35,6 +35,12 @@
   </si>
   <si>
     <t xml:space="preserve">Height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test2</t>
   </si>
   <si>
     <t xml:space="preserve">Adam Smith</t>
@@ -133,16 +139,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -269,78 +271,93 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="4.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="6.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="n">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>12345</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>4567</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2" t="n">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>8787</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>999</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
feat(userinfo): adding output to the console to inform the user of the steps being taken
</commit_message>
<xml_diff>
--- a/Data/ExcelBeginner.xlsx
+++ b/Data/ExcelBeginner.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -35,12 +35,6 @@
   </si>
   <si>
     <t xml:space="preserve">Height</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test2</t>
   </si>
   <si>
     <t xml:space="preserve">Adam Smith</t>
@@ -271,10 +265,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -301,57 +295,39 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>12345</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>4567</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>35</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>8787</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>